<commit_message>
Updated BOM and output schematics
</commit_message>
<xml_diff>
--- a/hardware/Outputs/BOM/BOM.xlsx
+++ b/hardware/Outputs/BOM/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Documents\repos\EasyPlay\hardware\Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33174F-68C0-4F9A-96A8-27D10F7521FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D835EA6-7A95-4D69-BFAF-4C58DB13AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3996" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{417F7653-03C4-4A04-892D-459E4CFE0357}"/>
+    <workbookView xWindow="-636" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{82734134-AD62-4B7E-B2EC-FD89C8C8D21D}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="131">
   <si>
     <t>Library Reference</t>
   </si>
@@ -101,7 +101,7 @@
     <t>0.1uF, 50V, 0603</t>
   </si>
   <si>
-    <t>C1-MCU, C2-MCU, C2-PWR, C3-MCU, C4-MCU, C4-PWR, C5-MCU, C7-MCU</t>
+    <t>C1-CTRL, C1-MCU, C2-CTRL, C2-MCU, C2-PWR, C3-CTRL, C3-MCU, C4-MCU, C4-PWR, C5-MCU, C6-CTRL, C7-CTRL, C7-MCU</t>
   </si>
   <si>
     <t>MC0603N200J500CT</t>
@@ -143,7 +143,7 @@
     <t>10nF, 25V, 0603</t>
   </si>
   <si>
-    <t>C1-CTRL, C2-CTRL, C3-CTRL, C4-CTRL, C5-CTRL, C6-CTRL, C7-CTRL</t>
+    <t>C4-CTRL, C5-CTRL</t>
   </si>
   <si>
     <t>Cherry MX Switch</t>
@@ -311,19 +311,19 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>KOA</t>
-  </si>
-  <si>
-    <t>RK73H1JTTD1001F.</t>
-  </si>
-  <si>
-    <t>3548613</t>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>CR0603-FX-1001ELF</t>
+  </si>
+  <si>
+    <t>2008335</t>
   </si>
   <si>
     <t>1k, 100mW, 0603</t>
   </si>
   <si>
-    <t>R6-CTRL</t>
+    <t>R3-CTRL, R4-CTRL, R5-CTRL, R6-CTRL, R9-CTRL, R11-CTRL, R15-CTRL, R17-CTRL, R18-CTRL</t>
   </si>
   <si>
     <t>MC0805S8F0000T5E</t>
@@ -347,7 +347,19 @@
     <t>5.1k, 100mW, 0603</t>
   </si>
   <si>
-    <t>R1-CTRL, R2-CTRL, R3-CTRL, R4-CTRL, R5-CTRL, R5-USB, R6-USB, R7-CTRL, R8-CTRL, R9-CTRL, R10-CTRL, R11-CTRL, R12-CTRL, R13-CTRL, R14-CTRL, R15-CTRL, R16-CTRL, R17-CTRL, R18-CTRL</t>
+    <t>R5-USB, R6-USB</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>9238603</t>
+  </si>
+  <si>
+    <t>10k, 100mW, 0603</t>
+  </si>
+  <si>
+    <t>R8-CTRL, R10-CTRL, R12-CTRL, R13-CTRL</t>
   </si>
   <si>
     <t>RC0603FR-07270RL</t>
@@ -360,6 +372,18 @@
   </si>
   <si>
     <t>R1-MCU, R1-PWR, R2-MCU</t>
+  </si>
+  <si>
+    <t>RC0603FR-13100KL</t>
+  </si>
+  <si>
+    <t>2309107</t>
+  </si>
+  <si>
+    <t>100k, 100mW, 0603</t>
+  </si>
+  <si>
+    <t>R1-CTRL, R2-CTRL, R7-CTRL, R14-CTRL, R16-CTRL</t>
   </si>
   <si>
     <t>Rotary Encoder w/ Switch</t>
@@ -414,7 +438,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,15 +447,8 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,18 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,14 +489,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,12 +808,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8AD039-2AC4-4DED-ADB8-5D9CF32B3997}">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00839A2A-5C51-4C3F-9FCA-16EA468A5E53}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -824,602 +825,654 @@
     <col min="8" max="8" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="1">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="1">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="6">
-        <v>4</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="6">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="6">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="G23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="G24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>122</v>
+      <c r="G25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PCB passive component values (#2)
</commit_message>
<xml_diff>
--- a/hardware/Outputs/BOM/BOM.xlsx
+++ b/hardware/Outputs/BOM/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Documents\repos\EasyPlay\hardware\Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33174F-68C0-4F9A-96A8-27D10F7521FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D835EA6-7A95-4D69-BFAF-4C58DB13AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3996" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{417F7653-03C4-4A04-892D-459E4CFE0357}"/>
+    <workbookView xWindow="-636" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{82734134-AD62-4B7E-B2EC-FD89C8C8D21D}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="131">
   <si>
     <t>Library Reference</t>
   </si>
@@ -101,7 +101,7 @@
     <t>0.1uF, 50V, 0603</t>
   </si>
   <si>
-    <t>C1-MCU, C2-MCU, C2-PWR, C3-MCU, C4-MCU, C4-PWR, C5-MCU, C7-MCU</t>
+    <t>C1-CTRL, C1-MCU, C2-CTRL, C2-MCU, C2-PWR, C3-CTRL, C3-MCU, C4-MCU, C4-PWR, C5-MCU, C6-CTRL, C7-CTRL, C7-MCU</t>
   </si>
   <si>
     <t>MC0603N200J500CT</t>
@@ -143,7 +143,7 @@
     <t>10nF, 25V, 0603</t>
   </si>
   <si>
-    <t>C1-CTRL, C2-CTRL, C3-CTRL, C4-CTRL, C5-CTRL, C6-CTRL, C7-CTRL</t>
+    <t>C4-CTRL, C5-CTRL</t>
   </si>
   <si>
     <t>Cherry MX Switch</t>
@@ -311,19 +311,19 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>KOA</t>
-  </si>
-  <si>
-    <t>RK73H1JTTD1001F.</t>
-  </si>
-  <si>
-    <t>3548613</t>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>CR0603-FX-1001ELF</t>
+  </si>
+  <si>
+    <t>2008335</t>
   </si>
   <si>
     <t>1k, 100mW, 0603</t>
   </si>
   <si>
-    <t>R6-CTRL</t>
+    <t>R3-CTRL, R4-CTRL, R5-CTRL, R6-CTRL, R9-CTRL, R11-CTRL, R15-CTRL, R17-CTRL, R18-CTRL</t>
   </si>
   <si>
     <t>MC0805S8F0000T5E</t>
@@ -347,7 +347,19 @@
     <t>5.1k, 100mW, 0603</t>
   </si>
   <si>
-    <t>R1-CTRL, R2-CTRL, R3-CTRL, R4-CTRL, R5-CTRL, R5-USB, R6-USB, R7-CTRL, R8-CTRL, R9-CTRL, R10-CTRL, R11-CTRL, R12-CTRL, R13-CTRL, R14-CTRL, R15-CTRL, R16-CTRL, R17-CTRL, R18-CTRL</t>
+    <t>R5-USB, R6-USB</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>9238603</t>
+  </si>
+  <si>
+    <t>10k, 100mW, 0603</t>
+  </si>
+  <si>
+    <t>R8-CTRL, R10-CTRL, R12-CTRL, R13-CTRL</t>
   </si>
   <si>
     <t>RC0603FR-07270RL</t>
@@ -360,6 +372,18 @@
   </si>
   <si>
     <t>R1-MCU, R1-PWR, R2-MCU</t>
+  </si>
+  <si>
+    <t>RC0603FR-13100KL</t>
+  </si>
+  <si>
+    <t>2309107</t>
+  </si>
+  <si>
+    <t>100k, 100mW, 0603</t>
+  </si>
+  <si>
+    <t>R1-CTRL, R2-CTRL, R7-CTRL, R14-CTRL, R16-CTRL</t>
   </si>
   <si>
     <t>Rotary Encoder w/ Switch</t>
@@ -414,7 +438,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,15 +447,8 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,18 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,14 +489,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,12 +808,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8AD039-2AC4-4DED-ADB8-5D9CF32B3997}">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00839A2A-5C51-4C3F-9FCA-16EA468A5E53}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -824,602 +825,654 @@
     <col min="8" max="8" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="1">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="1">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="6">
-        <v>4</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="6">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="6">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="G23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="G24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>122</v>
+      <c r="G25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>